<commit_message>
Batman The Dark Knight
</commit_message>
<xml_diff>
--- a/Creators.xlsx
+++ b/Creators.xlsx
@@ -8629,6 +8629,9 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="__Anonymous_Sheet_DB__0" displayName="__Anonymous_Sheet_DB__0" ref="C2:F177" headerRowCount="0" totalsRowShown="0">
+  <sortState ref="C2:D177">
+    <sortCondition ref="C2"/>
+  </sortState>
   <tableColumns count="4">
     <tableColumn id="1" name="Column1"/>
     <tableColumn id="2" name="Column2"/>
@@ -8904,8 +8907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C132" sqref="C132"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A150" sqref="A150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9449,7 +9452,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C67" t="s">
         <v>133</v>
@@ -9457,7 +9460,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C68" t="s">
         <v>135</v>
@@ -9465,7 +9468,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C69" t="s">
         <v>137</v>
@@ -9473,7 +9476,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C70" t="s">
         <v>139</v>
@@ -9481,7 +9484,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C71" t="s">
         <v>141</v>
@@ -9489,7 +9492,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C72" t="s">
         <v>143</v>
@@ -9497,7 +9500,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C73" t="s">
         <v>145</v>
@@ -9505,7 +9508,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C74" t="s">
         <v>147</v>
@@ -9513,7 +9516,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C75" t="s">
         <v>149</v>
@@ -9521,7 +9524,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C76" t="s">
         <v>151</v>
@@ -9529,7 +9532,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C77" t="s">
         <v>153</v>
@@ -9537,7 +9540,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C78" t="s">
         <v>155</v>
@@ -9545,7 +9548,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C79" t="s">
         <v>157</v>
@@ -9553,7 +9556,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C80" t="s">
         <v>159</v>
@@ -9561,7 +9564,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C81" t="s">
         <v>161</v>
@@ -9569,7 +9572,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C82" t="s">
         <v>163</v>
@@ -9577,7 +9580,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C83" t="s">
         <v>165</v>
@@ -9585,7 +9588,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C84" t="s">
         <v>167</v>
@@ -9593,7 +9596,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C85" t="s">
         <v>169</v>
@@ -9601,7 +9604,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C86" t="s">
         <v>171</v>
@@ -9609,7 +9612,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C87" t="s">
         <v>173</v>
@@ -9617,7 +9620,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C88" t="s">
         <v>175</v>
@@ -9625,7 +9628,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C89" t="s">
         <v>177</v>
@@ -9633,521 +9636,513 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C90" t="s">
-        <v>179</v>
+        <v>132</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C91" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C92" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C93" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C94" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B95" s="3"/>
       <c r="C95" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B96" s="5"/>
       <c r="C96" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C97" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C98" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C99" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C100" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C101" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A102" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="C102" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A103" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="C103" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>208</v>
+      </c>
+      <c r="C104" t="s">
         <v>201</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A102" t="s">
-        <v>202</v>
-      </c>
-      <c r="C102" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A103" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="C103" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A104" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="C104" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="C105" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
+        <v>214</v>
+      </c>
       <c r="C106" t="s">
-        <v>211</v>
+        <v>248</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="C107" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="C108" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="C109" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="C110" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="C111" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="C112" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="C113" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="C114" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="C115" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="C116" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="C117" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="C118" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="C119" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="C120" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="C121" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>242</v>
+        <v>250</v>
       </c>
       <c r="C122" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
       <c r="C123" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="B124" s="3"/>
       <c r="C124" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="C125" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>250</v>
+        <v>258</v>
       </c>
       <c r="C126" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>252</v>
+        <v>260</v>
       </c>
       <c r="C127" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>254</v>
+        <v>262</v>
       </c>
       <c r="C128" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
       <c r="C129" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A130" t="s">
-        <v>258</v>
+      <c r="A130" s="3" t="s">
+        <v>264</v>
       </c>
       <c r="C130" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="C131" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="C132" t="s">
-        <v>210</v>
+        <v>255</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>263</v>
+        <v>267</v>
+      </c>
+      <c r="C133" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A134" s="3" t="s">
-        <v>264</v>
+      <c r="A134" t="s">
+        <v>268</v>
+      </c>
+      <c r="C134" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>265</v>
+        <v>269</v>
+      </c>
+      <c r="C135" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="B154" s="3"/>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A162" t="s">
-        <v>292</v>
+      <c r="A162" s="3" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A164" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A165" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A166" s="3" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A167" t="s">
         <v>297</v>
       </c>
     </row>
@@ -10155,6 +10150,9 @@
       <c r="D177" s="6"/>
     </row>
   </sheetData>
+  <sortState ref="A2:A167">
+    <sortCondition ref="A2"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="1.14375" bottom="1.14375" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
@@ -11356,10 +11354,10 @@
     <hyperlink ref="A93" r:id="rId93"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId94"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P&amp;L&amp;1#&amp;"Calibri"&amp;6&amp;K7F7F7FInternal Use - Confidential</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -11888,7 +11886,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;1#&amp;"Calibri"&amp;6&amp;K7F7F7FInternal Use - Confidential</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -12274,9 +12275,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
-    <oddFooter>&amp;L&amp;1#&amp;6Internal Use - Confidential</oddFooter>
+    <oddFooter>&amp;L&amp;1#&amp;"Calibri"&amp;6&amp;K7F7F7FInternal Use - Confidential</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -13700,10 +13701,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;L&amp;1#&amp;6Internal Use - Confidential&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P&amp;L&amp;1#&amp;"Calibri"&amp;6&amp;K7F7F7FInternal Use - Confidential</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -18858,9 +18859,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
-    <oddFooter>&amp;L&amp;1#&amp;6Internal Use - Confidential</oddFooter>
+    <oddFooter>&amp;L&amp;1#&amp;"Calibri"&amp;6&amp;K7F7F7FInternal Use - Confidential</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -19160,10 +19161,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;L&amp;1#&amp;6Internal Use - Confidential&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P&amp;L&amp;1#&amp;"Calibri"&amp;6&amp;K7F7F7FInternal Use - Confidential</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -25088,9 +25089,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
-    <oddFooter>&amp;L&amp;1#&amp;6Internal Use - Confidential</oddFooter>
+    <oddFooter>&amp;L&amp;1#&amp;"Calibri"&amp;6&amp;K7F7F7FInternal Use - Confidential</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -25455,9 +25456,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
-    <oddFooter>&amp;L&amp;1#&amp;6Internal Use - Confidential</oddFooter>
+    <oddFooter>&amp;L&amp;1#&amp;"Calibri"&amp;6&amp;K7F7F7FInternal Use - Confidential</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -27805,10 +27806,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;L&amp;1#&amp;6Internal Use - Confidential&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P&amp;L&amp;1#&amp;"Calibri"&amp;6&amp;K7F7F7FInternal Use - Confidential</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -28041,9 +28042,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
-    <oddFooter>&amp;L&amp;1#&amp;6Internal Use - Confidential</oddFooter>
+    <oddFooter>&amp;L&amp;1#&amp;"Calibri"&amp;6&amp;K7F7F7FInternal Use - Confidential</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>